<commit_message>
remove entity from enemies if the enemy is on deathTimer upon deserialization
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive - UBC\UBC\Courses\Year 4\CPSC 427\MainRepo\Team17\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53A79A1-ACBE-4E7C-93DD-EEFFFFA6FFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E682B733-4230-4E69-AF99-BED98A2A4158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="91">
   <si>
     <t>Bug List</t>
   </si>
@@ -258,17 +258,60 @@
   </si>
   <si>
     <t>Press P to pause the game and then, Press H to go to Help Menu.</t>
+  </si>
+  <si>
+    <t>Knocked enemies don't stop when they hit the ground</t>
+  </si>
+  <si>
+    <t>Knocked enemies should stop momentarily when they hit the ground</t>
+  </si>
+  <si>
+    <t>Knocked enemies should stop for a while when they hit the ground</t>
+  </si>
+  <si>
+    <t>Try to get "Troll" enemy to knock other entities</t>
+  </si>
+  <si>
+    <t>Repeatedly jumping  consumes stamina</t>
+  </si>
+  <si>
+    <t>Repeatedly jumping should continue consuming stamina</t>
+  </si>
+  <si>
+    <t>Repeatedly jumping by holding space bar does not continue consuming stamina</t>
+  </si>
+  <si>
+    <t>Press space for as long as there is enough stamina to jump</t>
+  </si>
+  <si>
+    <t>Introduction of Phantom trap affects how traps are counted and serialized/deserialized, causing the main branch to fail.</t>
+  </si>
+  <si>
+    <t>The program should compile without errors.</t>
+  </si>
+  <si>
+    <t>The program compiles without errors.</t>
+  </si>
+  <si>
+    <t>Run the program.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -341,41 +384,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1097,103 +1141,184 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>13</v>
+      </c>
+      <c r="C16" s="13">
+        <v>45622</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>14</v>
+      </c>
+      <c r="C17" s="13">
+        <v>45614</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>15</v>
+      </c>
+      <c r="C18" s="13">
+        <v>45624</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>16</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H21" s="2"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H22" s="2"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H23" s="2"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H24" s="2"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H25" s="2"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H26" s="2"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H27" s="2"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H28" s="2"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
-    <row r="29" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H29" s="2"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H30" s="2"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
     </row>
-    <row r="31" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H31" s="2"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H32" s="2"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>

</xml_diff>

<commit_message>
add test plan & bug report
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documents\427\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53A79A1-ACBE-4E7C-93DD-EEFFFFA6FFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78112D3-B9AF-46BA-AFD4-2437E105C4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
   <si>
     <t>Bug List</t>
   </si>
@@ -167,12 +167,6 @@
     <t>Game should not have memory leaks</t>
   </si>
   <si>
-    <t>Memory leaks detected</t>
-  </si>
-  <si>
-    <t>Can be detected using Visual Studio's memory profiler</t>
-  </si>
-  <si>
     <t>Severity</t>
   </si>
   <si>
@@ -206,12 +200,6 @@
     <t>minor or feature that nice to have but could ship in future release</t>
   </si>
   <si>
-    <t>In-Progress</t>
-  </si>
-  <si>
-    <t>Some memory leaks detected using Visual Studio profiler and Deleaker.</t>
-  </si>
-  <si>
     <t>Spawning system could not handle negative initial values.</t>
   </si>
   <si>
@@ -258,17 +246,76 @@
   </si>
   <si>
     <t>Press P to pause the game and then, Press H to go to Help Menu.</t>
+  </si>
+  <si>
+    <t>Knocked enemies don't stop when they hit the ground</t>
+  </si>
+  <si>
+    <t>Knocked enemies should stop momentarily when they hit the ground</t>
+  </si>
+  <si>
+    <t>Knocked enemies should stop for a while when they hit the ground</t>
+  </si>
+  <si>
+    <t>Try to get "Troll" enemy to knock other entities</t>
+  </si>
+  <si>
+    <t>Repeatedly jumping  consumes stamina</t>
+  </si>
+  <si>
+    <t>Repeatedly jumping should continue consuming stamina</t>
+  </si>
+  <si>
+    <t>Repeatedly jumping by holding space bar does not continue consuming stamina</t>
+  </si>
+  <si>
+    <t>Press space for as long as there is enough stamina to jump</t>
+  </si>
+  <si>
+    <t>Introduction of Phantom trap affects how traps are counted and serialized/deserialized, causing the main branch to fail.</t>
+  </si>
+  <si>
+    <t>The program should compile without errors.</t>
+  </si>
+  <si>
+    <t>The program compiles without errors.</t>
+  </si>
+  <si>
+    <t>Run the program.</t>
+  </si>
+  <si>
+    <t>Can use Visual Studio Profiler</t>
+  </si>
+  <si>
+    <t>No memory leaks other than template leaks.</t>
+  </si>
+  <si>
+    <t>No memory leaks other than template leaks detected using Visual Studio profiler and Deleaker.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -341,40 +388,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -929,7 +981,7 @@
       <c r="B11" s="9">
         <v>3</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="11">
         <v>45602</v>
       </c>
       <c r="D11" s="9" t="s">
@@ -944,17 +996,17 @@
       <c r="G11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>70</v>
+      <c r="H11" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -964,14 +1016,14 @@
       <c r="B12" s="9">
         <v>3</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>45602</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>14</v>
@@ -979,17 +1031,17 @@
       <c r="G12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>74</v>
+      <c r="H12" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -999,7 +1051,7 @@
       <c r="B13" s="9">
         <v>3</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>45610</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -1014,17 +1066,17 @@
       <c r="G13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>78</v>
+      <c r="H13" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1034,7 +1086,7 @@
       <c r="B14" s="9">
         <v>3</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>45612</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -1049,20 +1101,20 @@
       <c r="G14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -1078,122 +1130,201 @@
       <c r="E15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>61</v>
+      <c r="F15" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" s="12" t="s">
+      <c r="H15" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J15" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>13</v>
+      </c>
+      <c r="C16" s="11">
+        <v>45622</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>14</v>
+      </c>
+      <c r="C17" s="11">
+        <v>45614</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>15</v>
+      </c>
+      <c r="C18" s="11">
+        <v>45624</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
       <c r="H19" s="2"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H21" s="2"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H22" s="2"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H23" s="2"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H24" s="2"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H25" s="2"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H26" s="2"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H27" s="2"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H28" s="2"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
-    <row r="29" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H29" s="2"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H30" s="2"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
     </row>
-    <row r="31" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H31" s="2"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="8:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H32" s="2"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -7014,10 +7145,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7025,23 +7156,23 @@
         <v>20</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7049,7 +7180,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7057,15 +7188,15 @@
         <v>29</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>